<commit_message>
update results for results_v1.txt
</commit_message>
<xml_diff>
--- a/stl/results_filter_excel.xlsx
+++ b/stl/results_filter_excel.xlsx
@@ -47,52 +47,52 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00752125"/>
+        <fgColor rgb="00767941"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00719536"/>
+        <fgColor rgb="00700453"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00708950"/>
+        <fgColor rgb="00754730"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00725184"/>
+        <fgColor rgb="00733783"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00717139"/>
+        <fgColor rgb="00745861"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00704319"/>
+        <fgColor rgb="00741710"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00766011"/>
+        <fgColor rgb="00744213"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00752727"/>
+        <fgColor rgb="00705466"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00746267"/>
+        <fgColor rgb="00731738"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00717733"/>
+        <fgColor rgb="00750877"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>

<commit_message>
confirmed results for script_diff_one_v2.2.txt
</commit_message>
<xml_diff>
--- a/stl/results_filter_excel.xlsx
+++ b/stl/results_filter_excel.xlsx
@@ -47,52 +47,52 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00742607"/>
+        <fgColor rgb="00703736"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00737717"/>
+        <fgColor rgb="00767888"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00777325"/>
+        <fgColor rgb="00724424"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00750509"/>
+        <fgColor rgb="00741845"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00763468"/>
+        <fgColor rgb="00760111"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00724874"/>
+        <fgColor rgb="00735682"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00717465"/>
+        <fgColor rgb="00719043"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00748343"/>
+        <fgColor rgb="00745198"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00771311"/>
+        <fgColor rgb="00754577"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00753883"/>
+        <fgColor rgb="00768171"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>

<commit_message>
fix seq_type bug giving off different diff_two results. created script_diff_one_v2.3.py
</commit_message>
<xml_diff>
--- a/stl/results_filter_excel.xlsx
+++ b/stl/results_filter_excel.xlsx
@@ -47,52 +47,52 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00751287"/>
+        <fgColor rgb="00710085"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00715078"/>
+        <fgColor rgb="00730965"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00703386"/>
+        <fgColor rgb="00729850"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00727869"/>
+        <fgColor rgb="00746960"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00767036"/>
+        <fgColor rgb="00752131"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00761855"/>
+        <fgColor rgb="00730932"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00759049"/>
+        <fgColor rgb="00747687"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00758676"/>
+        <fgColor rgb="00750116"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00729829"/>
+        <fgColor rgb="00723324"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00733937"/>
+        <fgColor rgb="00700616"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>

<commit_message>
update results and probables; delete demo.py
</commit_message>
<xml_diff>
--- a/stl/results_filter_excel.xlsx
+++ b/stl/results_filter_excel.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -47,52 +47,52 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00764267"/>
+        <fgColor rgb="00708816"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00704285"/>
+        <fgColor rgb="00737422"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00764520"/>
+        <fgColor rgb="00727269"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00704943"/>
+        <fgColor rgb="00707397"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00715299"/>
+        <fgColor rgb="00727658"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00778506"/>
+        <fgColor rgb="00772409"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00745696"/>
+        <fgColor rgb="00762375"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00751242"/>
+        <fgColor rgb="00753419"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00712962"/>
+        <fgColor rgb="00733753"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00770051"/>
+        <fgColor rgb="00714093"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>